<commit_message>
Last commit before moving to new repo
</commit_message>
<xml_diff>
--- a/research/Pawn Instructions.xlsx
+++ b/research/Pawn Instructions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\Projects\PokeRandomizer\research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1C510DE-0990-4361-95AC-D093F9236FE1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E0A7BA4-7DFE-4BD6-851D-23961EF57BC1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FF7356ED-52C7-4695-8F1B-4A5374065396}"/>
   </bookViews>
@@ -1322,13 +1322,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{29F4215C-045C-4FF1-BBCD-5A60B8D71A8C}" name="Table1" displayName="Table1" ref="A1:H176" totalsRowShown="0" headerRowDxfId="4" headerRowBorderDxfId="6">
-  <autoFilter ref="A1:H176" xr:uid="{6B447A6B-333D-4067-A86F-BB98FB240C72}">
-    <filterColumn colId="6">
-      <filters>
-        <filter val="#REF!"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:H176" xr:uid="{6B447A6B-333D-4067-A86F-BB98FB240C72}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{7CD61093-5B47-4064-9A71-6BE9C709D03C}" name="OPCODE" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{DB059D25-6A84-4CC2-866B-8E5571A54002}" name="NAME" dataDxfId="3"/>
@@ -1648,8 +1642,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1BA90AF-E104-45A4-8D26-E0CF7E73167E}">
   <dimension ref="A1:J176"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F82" sqref="F82"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1691,7 +1685,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="2" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
         <v>0</v>
       </c>
@@ -1717,7 +1711,7 @@
         <v>{ AmxOpCode.NOP, AmxOpCodeType.NoParams },</v>
       </c>
     </row>
-    <row r="3" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <v>1</v>
       </c>
@@ -1746,7 +1740,7 @@
         <v>{ AmxOpCode.LOAD_PRI, AmxOpCodeType.OneParam },</v>
       </c>
     </row>
-    <row r="4" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <v>2</v>
       </c>
@@ -1775,7 +1769,7 @@
         <v>{ AmxOpCode.LOAD_ALT, AmxOpCodeType.OneParam },</v>
       </c>
     </row>
-    <row r="5" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>3</v>
       </c>
@@ -1804,7 +1798,7 @@
         <v>{ AmxOpCode.LOAD_S_PRI, AmxOpCodeType.OneParam },</v>
       </c>
     </row>
-    <row r="6" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>4</v>
       </c>
@@ -1833,7 +1827,7 @@
         <v>{ AmxOpCode.LOAD_S_ALT, AmxOpCodeType.OneParam },</v>
       </c>
     </row>
-    <row r="7" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>5</v>
       </c>
@@ -1862,7 +1856,7 @@
         <v>{ AmxOpCode.LREF_S_PRI, AmxOpCodeType.OneParam },</v>
       </c>
     </row>
-    <row r="8" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <v>6</v>
       </c>
@@ -1891,7 +1885,7 @@
         <v>{ AmxOpCode.LREF_S_ALT, AmxOpCodeType.OneParam },</v>
       </c>
     </row>
-    <row r="9" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <v>7</v>
       </c>
@@ -1920,7 +1914,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="10" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <v>8</v>
       </c>
@@ -1952,7 +1946,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="11" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <v>9</v>
       </c>
@@ -1984,7 +1978,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="12" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
         <v>10</v>
       </c>
@@ -2016,7 +2010,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="13" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
         <v>11</v>
       </c>
@@ -2048,7 +2042,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="14" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
         <v>12</v>
       </c>
@@ -2080,7 +2074,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="15" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
         <v>13</v>
       </c>
@@ -2112,7 +2106,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="16" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
         <v>14</v>
       </c>
@@ -2144,7 +2138,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="17" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
         <v>15</v>
       </c>
@@ -2176,7 +2170,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="18" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
         <v>16</v>
       </c>
@@ -2202,7 +2196,7 @@
         <v>{ AmxOpCode.STOR_I, AmxOpCodeType.NoParams },</v>
       </c>
     </row>
-    <row r="19" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
         <v>17</v>
       </c>
@@ -2231,7 +2225,7 @@
         <v>{ AmxOpCode.STRB_I, AmxOpCodeType.OneParam },</v>
       </c>
     </row>
-    <row r="20" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="8">
         <v>18</v>
       </c>
@@ -2260,7 +2254,7 @@
         <v>{ AmxOpCode.ALIGN_PRI, AmxOpCodeType.OneParam },</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
         <v>19</v>
       </c>
@@ -2289,7 +2283,7 @@
         <v>{ AmxOpCode.LCTRL, AmxOpCodeType.OneParam },</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="8">
         <v>20</v>
       </c>
@@ -2318,7 +2312,7 @@
         <v>{ AmxOpCode.SCTRL, AmxOpCodeType.OneParam },</v>
       </c>
     </row>
-    <row r="23" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
         <v>21</v>
       </c>
@@ -2344,7 +2338,7 @@
         <v>{ AmxOpCode.XCHG, AmxOpCodeType.NoParams },</v>
       </c>
     </row>
-    <row r="24" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="8">
         <v>22</v>
       </c>
@@ -2370,7 +2364,7 @@
         <v>{ AmxOpCode.PUSH_PRI, AmxOpCodeType.NoParams },</v>
       </c>
     </row>
-    <row r="25" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="8">
         <v>23</v>
       </c>
@@ -2396,7 +2390,7 @@
         <v>{ AmxOpCode.PUSH_ALT, AmxOpCodeType.NoParams },</v>
       </c>
     </row>
-    <row r="26" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="8">
         <v>24</v>
       </c>
@@ -2422,7 +2416,7 @@
         <v>{ AmxOpCode.PUSHR_PRI, AmxOpCodeType.NoParams },</v>
       </c>
     </row>
-    <row r="27" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="8">
         <v>25</v>
       </c>
@@ -2448,7 +2442,7 @@
         <v>{ AmxOpCode.POP_PRI, AmxOpCodeType.NoParams },</v>
       </c>
     </row>
-    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="8">
         <v>26</v>
       </c>
@@ -2474,7 +2468,7 @@
         <v>{ AmxOpCode.POP_ALT, AmxOpCodeType.NoParams },</v>
       </c>
     </row>
-    <row r="29" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="8">
         <v>27</v>
       </c>
@@ -2503,7 +2497,7 @@
         <v>{ AmxOpCode.PICK, AmxOpCodeType.OneParam },</v>
       </c>
     </row>
-    <row r="30" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="8">
         <v>28</v>
       </c>
@@ -2532,7 +2526,7 @@
         <v>{ AmxOpCode.STACK, AmxOpCodeType.OneParam },</v>
       </c>
     </row>
-    <row r="31" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="8">
         <v>29</v>
       </c>
@@ -2561,7 +2555,7 @@
         <v>{ AmxOpCode.HEAP, AmxOpCodeType.OneParam },</v>
       </c>
     </row>
-    <row r="32" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="8">
         <v>30</v>
       </c>
@@ -2587,7 +2581,7 @@
         <v>{ AmxOpCode.PROC, AmxOpCodeType.NoParams },</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="8">
         <v>31</v>
       </c>
@@ -2613,7 +2607,7 @@
         <v>{ AmxOpCode.RET, AmxOpCodeType.NoParams },</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A34" s="8">
         <v>32</v>
       </c>
@@ -2639,7 +2633,7 @@
         <v>{ AmxOpCode.RETN, AmxOpCodeType.NoParams },</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A35" s="8">
         <v>33</v>
       </c>
@@ -2668,7 +2662,7 @@
         <v>{ AmxOpCode.CALL, AmxOpCodeType.Jump },</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="8">
         <v>34</v>
       </c>
@@ -2697,7 +2691,7 @@
         <v>{ AmxOpCode.JUMP, AmxOpCodeType.Jump },</v>
       </c>
     </row>
-    <row r="37" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="8">
         <v>35</v>
       </c>
@@ -2726,7 +2720,7 @@
         <v>{ AmxOpCode.JZER, AmxOpCodeType.Jump },</v>
       </c>
     </row>
-    <row r="38" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="8">
         <v>36</v>
       </c>
@@ -2755,7 +2749,7 @@
         <v>{ AmxOpCode.JNZ, AmxOpCodeType.Jump },</v>
       </c>
     </row>
-    <row r="39" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="8">
         <v>37</v>
       </c>
@@ -2781,7 +2775,7 @@
         <v>{ AmxOpCode.SHL, AmxOpCodeType.NoParams },</v>
       </c>
     </row>
-    <row r="40" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="8">
         <v>38</v>
       </c>
@@ -2807,7 +2801,7 @@
         <v>{ AmxOpCode.SHR, AmxOpCodeType.NoParams },</v>
       </c>
     </row>
-    <row r="41" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="8">
         <v>39</v>
       </c>
@@ -2833,7 +2827,7 @@
         <v>{ AmxOpCode.SSHR, AmxOpCodeType.NoParams },</v>
       </c>
     </row>
-    <row r="42" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="8">
         <v>40</v>
       </c>
@@ -2862,7 +2856,7 @@
         <v>{ AmxOpCode.SHL_C_PRI, AmxOpCodeType.OneParam },</v>
       </c>
     </row>
-    <row r="43" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="8">
         <v>41</v>
       </c>
@@ -2891,7 +2885,7 @@
         <v>{ AmxOpCode.SHL_C_ALT, AmxOpCodeType.OneParam },</v>
       </c>
     </row>
-    <row r="44" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="8">
         <v>42</v>
       </c>
@@ -2917,7 +2911,7 @@
         <v>{ AmxOpCode.SMUL, AmxOpCodeType.NoParams },</v>
       </c>
     </row>
-    <row r="45" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="8">
         <v>43</v>
       </c>
@@ -2943,7 +2937,7 @@
         <v>{ AmxOpCode.SDIV, AmxOpCodeType.NoParams },</v>
       </c>
     </row>
-    <row r="46" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="8">
         <v>44</v>
       </c>
@@ -2969,7 +2963,7 @@
         <v>{ AmxOpCode.ADD, AmxOpCodeType.NoParams },</v>
       </c>
     </row>
-    <row r="47" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="8">
         <v>45</v>
       </c>
@@ -2995,7 +2989,7 @@
         <v>{ AmxOpCode.SUB, AmxOpCodeType.NoParams },</v>
       </c>
     </row>
-    <row r="48" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="8">
         <v>46</v>
       </c>
@@ -3021,7 +3015,7 @@
         <v>{ AmxOpCode.AND, AmxOpCodeType.NoParams },</v>
       </c>
     </row>
-    <row r="49" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="8">
         <v>47</v>
       </c>
@@ -3047,7 +3041,7 @@
         <v>{ AmxOpCode.OR, AmxOpCodeType.NoParams },</v>
       </c>
     </row>
-    <row r="50" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="8">
         <v>48</v>
       </c>
@@ -3073,7 +3067,7 @@
         <v>{ AmxOpCode.XOR, AmxOpCodeType.NoParams },</v>
       </c>
     </row>
-    <row r="51" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="8">
         <v>49</v>
       </c>
@@ -3099,7 +3093,7 @@
         <v>{ AmxOpCode.NOT, AmxOpCodeType.NoParams },</v>
       </c>
     </row>
-    <row r="52" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="8">
         <v>50</v>
       </c>
@@ -3125,7 +3119,7 @@
         <v>{ AmxOpCode.NEG, AmxOpCodeType.NoParams },</v>
       </c>
     </row>
-    <row r="53" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="8">
         <v>51</v>
       </c>
@@ -3151,7 +3145,7 @@
         <v>{ AmxOpCode.INVERT, AmxOpCodeType.NoParams },</v>
       </c>
     </row>
-    <row r="54" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="8">
         <v>52</v>
       </c>
@@ -3177,7 +3171,7 @@
         <v>{ AmxOpCode.EQ, AmxOpCodeType.NoParams },</v>
       </c>
     </row>
-    <row r="55" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="8">
         <v>53</v>
       </c>
@@ -3203,7 +3197,7 @@
         <v>{ AmxOpCode.NEQ, AmxOpCodeType.NoParams },</v>
       </c>
     </row>
-    <row r="56" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="8">
         <v>54</v>
       </c>
@@ -3229,7 +3223,7 @@
         <v>{ AmxOpCode.SLESS, AmxOpCodeType.NoParams },</v>
       </c>
     </row>
-    <row r="57" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="8">
         <v>55</v>
       </c>
@@ -3255,7 +3249,7 @@
         <v>{ AmxOpCode.SLEQ, AmxOpCodeType.NoParams },</v>
       </c>
     </row>
-    <row r="58" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="8">
         <v>56</v>
       </c>
@@ -3281,7 +3275,7 @@
         <v>{ AmxOpCode.SGRTR, AmxOpCodeType.NoParams },</v>
       </c>
     </row>
-    <row r="59" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="8">
         <v>57</v>
       </c>
@@ -3307,7 +3301,7 @@
         <v>{ AmxOpCode.SGEQ, AmxOpCodeType.NoParams },</v>
       </c>
     </row>
-    <row r="60" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="8">
         <v>58</v>
       </c>
@@ -3333,7 +3327,7 @@
         <v>{ AmxOpCode.INC_PRI, AmxOpCodeType.NoParams },</v>
       </c>
     </row>
-    <row r="61" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="8">
         <v>59</v>
       </c>
@@ -3359,7 +3353,7 @@
         <v>{ AmxOpCode.INC_ALT, AmxOpCodeType.NoParams },</v>
       </c>
     </row>
-    <row r="62" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="8">
         <v>60</v>
       </c>
@@ -3385,7 +3379,7 @@
         <v>{ AmxOpCode.INC_I, AmxOpCodeType.NoParams },</v>
       </c>
     </row>
-    <row r="63" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="8">
         <v>61</v>
       </c>
@@ -3411,7 +3405,7 @@
         <v>{ AmxOpCode.DEC_PRI, AmxOpCodeType.NoParams },</v>
       </c>
     </row>
-    <row r="64" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="8">
         <v>62</v>
       </c>
@@ -3437,7 +3431,7 @@
         <v>{ AmxOpCode.DEC_ALT, AmxOpCodeType.NoParams },</v>
       </c>
     </row>
-    <row r="65" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="8">
         <v>63</v>
       </c>
@@ -3463,7 +3457,7 @@
         <v>{ AmxOpCode.DEC_I, AmxOpCodeType.NoParams },</v>
       </c>
     </row>
-    <row r="66" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A66" s="8">
         <v>64</v>
       </c>
@@ -3492,7 +3486,7 @@
         <v>{ AmxOpCode.MOVS, AmxOpCodeType.OneParam },</v>
       </c>
     </row>
-    <row r="67" spans="1:8" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A67" s="8">
         <v>65</v>
       </c>
@@ -3521,7 +3515,7 @@
         <v>{ AmxOpCode.CMPS, AmxOpCodeType.OneParam },</v>
       </c>
     </row>
-    <row r="68" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" s="8">
         <v>66</v>
       </c>
@@ -3550,7 +3544,7 @@
         <v>{ AmxOpCode.FILL, AmxOpCodeType.OneParam },</v>
       </c>
     </row>
-    <row r="69" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A69" s="8">
         <v>67</v>
       </c>
@@ -3579,7 +3573,7 @@
         <v>{ AmxOpCode.HALT, AmxOpCodeType.OneParam },</v>
       </c>
     </row>
-    <row r="70" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="8">
         <v>68</v>
       </c>
@@ -3608,7 +3602,7 @@
         <v>{ AmxOpCode.BOUNDS, AmxOpCodeType.OneParam },</v>
       </c>
     </row>
-    <row r="71" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="8">
         <v>69</v>
       </c>
@@ -3637,7 +3631,7 @@
         <v>{ AmxOpCode.SYSREQ, AmxOpCodeType.OneParam },</v>
       </c>
     </row>
-    <row r="72" spans="1:8" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A72" s="8">
         <v>70</v>
       </c>
@@ -3666,7 +3660,7 @@
         <v>{ AmxOpCode.SWITCH, AmxOpCodeType.Jump },</v>
       </c>
     </row>
-    <row r="73" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="8">
         <v>71</v>
       </c>
@@ -3692,7 +3686,7 @@
         <v>{ AmxOpCode.SWAP_PRI, AmxOpCodeType.NoParams },</v>
       </c>
     </row>
-    <row r="74" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="8">
         <v>72</v>
       </c>
@@ -3718,7 +3712,7 @@
         <v>{ AmxOpCode.SWAP_ALT, AmxOpCodeType.NoParams },</v>
       </c>
     </row>
-    <row r="75" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="8">
         <v>73</v>
       </c>
@@ -3773,7 +3767,7 @@
         <v>{ AmxOpCode.CASETBL, AmxOpCodeType.CaseTable },</v>
       </c>
     </row>
-    <row r="77" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="8">
         <v>75</v>
       </c>
@@ -3799,7 +3793,7 @@
         <v>{ AmxOpCode.SYSREQ_D, AmxOpCodeType.OneParam },</v>
       </c>
     </row>
-    <row r="78" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="8">
         <v>76</v>
       </c>
@@ -3825,7 +3819,7 @@
         <v>{ AmxOpCode.SYSREQ_ND, AmxOpCodeType.TwoParams },</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A79" s="8">
         <v>77</v>
       </c>
@@ -3854,7 +3848,7 @@
         <v>{ AmxOpCode.CALL_OVL, AmxOpCodeType.Jump },</v>
       </c>
     </row>
-    <row r="80" spans="1:8" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A80" s="8">
         <v>78</v>
       </c>
@@ -3880,7 +3874,7 @@
         <v>{ AmxOpCode.RETN_OVL, AmxOpCodeType.NoParams },</v>
       </c>
     </row>
-    <row r="81" spans="1:8" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A81" s="8">
         <v>79</v>
       </c>
@@ -3938,7 +3932,7 @@
         <v>{ AmxOpCode.CASETBL_OVL, AmxOpCodeType.CaseTable },</v>
       </c>
     </row>
-    <row r="83" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="8">
         <v>81</v>
       </c>
@@ -3964,7 +3958,7 @@
         <v>{ AmxOpCode.LIDX, AmxOpCodeType.NoParams },</v>
       </c>
     </row>
-    <row r="84" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="8">
         <v>82</v>
       </c>
@@ -3993,7 +3987,7 @@
         <v>{ AmxOpCode.LIDX_B, AmxOpCodeType.OneParam },</v>
       </c>
     </row>
-    <row r="85" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="8">
         <v>83</v>
       </c>
@@ -4019,7 +4013,7 @@
         <v>{ AmxOpCode.IDXADDR, AmxOpCodeType.NoParams },</v>
       </c>
     </row>
-    <row r="86" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="8">
         <v>84</v>
       </c>
@@ -4048,7 +4042,7 @@
         <v>{ AmxOpCode.IDXADDR_B, AmxOpCodeType.OneParam },</v>
       </c>
     </row>
-    <row r="87" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="8">
         <v>85</v>
       </c>
@@ -4077,7 +4071,7 @@
         <v>{ AmxOpCode.PUSH_C, AmxOpCodeType.OneParam },</v>
       </c>
     </row>
-    <row r="88" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="8">
         <v>86</v>
       </c>
@@ -4106,7 +4100,7 @@
         <v>{ AmxOpCode.PUSH, AmxOpCodeType.OneParam },</v>
       </c>
     </row>
-    <row r="89" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="8">
         <v>87</v>
       </c>
@@ -4135,7 +4129,7 @@
         <v>{ AmxOpCode.PUSH_S, AmxOpCodeType.OneParam },</v>
       </c>
     </row>
-    <row r="90" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="8">
         <v>88</v>
       </c>
@@ -4164,7 +4158,7 @@
         <v>{ AmxOpCode.PUSH_ADR, AmxOpCodeType.OneParam },</v>
       </c>
     </row>
-    <row r="91" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="8">
         <v>89</v>
       </c>
@@ -4193,7 +4187,7 @@
         <v>{ AmxOpCode.PUSHR_C, AmxOpCodeType.OneParam },</v>
       </c>
     </row>
-    <row r="92" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="8">
         <v>90</v>
       </c>
@@ -4222,7 +4216,7 @@
         <v>{ AmxOpCode.PUSHR_S, AmxOpCodeType.OneParam },</v>
       </c>
     </row>
-    <row r="93" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="8">
         <v>91</v>
       </c>
@@ -4251,7 +4245,7 @@
         <v>{ AmxOpCode.PUSHR_ADR, AmxOpCodeType.OneParam },</v>
       </c>
     </row>
-    <row r="94" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="8">
         <v>92</v>
       </c>
@@ -4280,7 +4274,7 @@
         <v>{ AmxOpCode.JEQ, AmxOpCodeType.Jump },</v>
       </c>
     </row>
-    <row r="95" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="8">
         <v>93</v>
       </c>
@@ -4309,7 +4303,7 @@
         <v>{ AmxOpCode.JNEQ, AmxOpCodeType.Jump },</v>
       </c>
     </row>
-    <row r="96" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="8">
         <v>94</v>
       </c>
@@ -4338,7 +4332,7 @@
         <v>{ AmxOpCode.JSLESS, AmxOpCodeType.Jump },</v>
       </c>
     </row>
-    <row r="97" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="8">
         <v>95</v>
       </c>
@@ -4367,7 +4361,7 @@
         <v>{ AmxOpCode.JSLEQ, AmxOpCodeType.Jump },</v>
       </c>
     </row>
-    <row r="98" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="8">
         <v>96</v>
       </c>
@@ -4396,7 +4390,7 @@
         <v>{ AmxOpCode.JSGRTR, AmxOpCodeType.Jump },</v>
       </c>
     </row>
-    <row r="99" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="8">
         <v>97</v>
       </c>
@@ -4425,7 +4419,7 @@
         <v>{ AmxOpCode.JSGEQ, AmxOpCodeType.Jump },</v>
       </c>
     </row>
-    <row r="100" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="8">
         <v>98</v>
       </c>
@@ -4451,7 +4445,7 @@
         <v>{ AmxOpCode.SDIV_INV, AmxOpCodeType.NoParams },</v>
       </c>
     </row>
-    <row r="101" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="8">
         <v>99</v>
       </c>
@@ -4477,7 +4471,7 @@
         <v>{ AmxOpCode.SUB_INV, AmxOpCodeType.NoParams },</v>
       </c>
     </row>
-    <row r="102" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" s="8">
         <v>100</v>
       </c>
@@ -4506,7 +4500,7 @@
         <v>{ AmxOpCode.ADD_C, AmxOpCodeType.OneParam },</v>
       </c>
     </row>
-    <row r="103" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="8">
         <v>101</v>
       </c>
@@ -4535,7 +4529,7 @@
         <v>{ AmxOpCode.SMUL_C, AmxOpCodeType.OneParam },</v>
       </c>
     </row>
-    <row r="104" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" s="8">
         <v>102</v>
       </c>
@@ -4561,7 +4555,7 @@
         <v>{ AmxOpCode.ZERO_PRI, AmxOpCodeType.NoParams },</v>
       </c>
     </row>
-    <row r="105" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="8">
         <v>103</v>
       </c>
@@ -4587,7 +4581,7 @@
         <v>{ AmxOpCode.ZERO_ALT, AmxOpCodeType.NoParams },</v>
       </c>
     </row>
-    <row r="106" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" s="8">
         <v>104</v>
       </c>
@@ -4616,7 +4610,7 @@
         <v>{ AmxOpCode.ZERO, AmxOpCodeType.OneParam },</v>
       </c>
     </row>
-    <row r="107" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" s="8">
         <v>105</v>
       </c>
@@ -4645,7 +4639,7 @@
         <v>{ AmxOpCode.ZERO_S, AmxOpCodeType.OneParam },</v>
       </c>
     </row>
-    <row r="108" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" s="8">
         <v>106</v>
       </c>
@@ -4674,7 +4668,7 @@
         <v>{ AmxOpCode.EQ_C_PRI, AmxOpCodeType.OneParam },</v>
       </c>
     </row>
-    <row r="109" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" s="8">
         <v>107</v>
       </c>
@@ -4703,7 +4697,7 @@
         <v>{ AmxOpCode.EQ_C_ALT, AmxOpCodeType.OneParam },</v>
       </c>
     </row>
-    <row r="110" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" s="8">
         <v>108</v>
       </c>
@@ -4732,7 +4726,7 @@
         <v>{ AmxOpCode.INC, AmxOpCodeType.OneParam },</v>
       </c>
     </row>
-    <row r="111" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" s="8">
         <v>109</v>
       </c>
@@ -4761,7 +4755,7 @@
         <v>{ AmxOpCode.INC_S, AmxOpCodeType.OneParam },</v>
       </c>
     </row>
-    <row r="112" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" s="8">
         <v>110</v>
       </c>
@@ -4790,7 +4784,7 @@
         <v>{ AmxOpCode.DEC, AmxOpCodeType.OneParam },</v>
       </c>
     </row>
-    <row r="113" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" s="8">
         <v>111</v>
       </c>
@@ -4819,7 +4813,7 @@
         <v>{ AmxOpCode.DEC_S, AmxOpCodeType.OneParam },</v>
       </c>
     </row>
-    <row r="114" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" s="8">
         <v>112</v>
       </c>
@@ -4848,7 +4842,7 @@
         <v>{ AmxOpCode.SYSREQ_N, AmxOpCodeType.OneParam },</v>
       </c>
     </row>
-    <row r="115" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" s="8">
         <v>113</v>
       </c>
@@ -4877,7 +4871,7 @@
         <v>{ AmxOpCode.PUSHM_C, AmxOpCodeType.NParams },</v>
       </c>
     </row>
-    <row r="116" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" s="8">
         <v>114</v>
       </c>
@@ -4906,7 +4900,7 @@
         <v>{ AmxOpCode.PUSHM, AmxOpCodeType.NParams },</v>
       </c>
     </row>
-    <row r="117" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" s="8">
         <v>115</v>
       </c>
@@ -4935,7 +4929,7 @@
         <v>{ AmxOpCode.PUSHM_S, AmxOpCodeType.NParams },</v>
       </c>
     </row>
-    <row r="118" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" s="8">
         <v>116</v>
       </c>
@@ -4964,7 +4958,7 @@
         <v>{ AmxOpCode.PUSHM_ADR, AmxOpCodeType.NParams },</v>
       </c>
     </row>
-    <row r="119" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" s="8">
         <v>117</v>
       </c>
@@ -4993,7 +4987,7 @@
         <v>{ AmxOpCode.PUSHRM_C, AmxOpCodeType.NParams },</v>
       </c>
     </row>
-    <row r="120" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" s="8">
         <v>118</v>
       </c>
@@ -5022,7 +5016,7 @@
         <v>{ AmxOpCode.PUSHRM_S, AmxOpCodeType.NParams },</v>
       </c>
     </row>
-    <row r="121" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121" s="8">
         <v>119</v>
       </c>
@@ -5051,7 +5045,7 @@
         <v>{ AmxOpCode.PUSHRM_ADR, AmxOpCodeType.NParams },</v>
       </c>
     </row>
-    <row r="122" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" s="8">
         <v>120</v>
       </c>
@@ -5080,7 +5074,7 @@
         <v>{ AmxOpCode.LOAD2, AmxOpCodeType.TwoParams },</v>
       </c>
     </row>
-    <row r="123" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123" s="8">
         <v>121</v>
       </c>
@@ -5109,7 +5103,7 @@
         <v>{ AmxOpCode.LOAD2_S, AmxOpCodeType.TwoParams },</v>
       </c>
     </row>
-    <row r="124" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124" s="8">
         <v>122</v>
       </c>
@@ -5138,7 +5132,7 @@
         <v>{ AmxOpCode.CONST, AmxOpCodeType.TwoParams },</v>
       </c>
     </row>
-    <row r="125" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" s="8">
         <v>123</v>
       </c>
@@ -5167,7 +5161,7 @@
         <v>{ AmxOpCode.CONST_S, AmxOpCodeType.TwoParams },</v>
       </c>
     </row>
-    <row r="126" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126" s="8">
         <v>124</v>
       </c>
@@ -5193,7 +5187,7 @@
         <v>{ AmxOpCode.LOAD_P_PRI, AmxOpCodeType.PackedOneParam },</v>
       </c>
     </row>
-    <row r="127" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127" s="8">
         <v>125</v>
       </c>
@@ -5219,7 +5213,7 @@
         <v>{ AmxOpCode.LOAD_P_ALT, AmxOpCodeType.PackedOneParam },</v>
       </c>
     </row>
-    <row r="128" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" s="8">
         <v>126</v>
       </c>
@@ -5245,7 +5239,7 @@
         <v>{ AmxOpCode.LOAD_P_S_PRI, AmxOpCodeType.PackedOneParam },</v>
       </c>
     </row>
-    <row r="129" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129" s="8">
         <v>127</v>
       </c>
@@ -5271,7 +5265,7 @@
         <v>{ AmxOpCode.LOAD_P_S_ALT, AmxOpCodeType.PackedOneParam },</v>
       </c>
     </row>
-    <row r="130" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130" s="8">
         <v>128</v>
       </c>
@@ -5297,7 +5291,7 @@
         <v>{ AmxOpCode.LREF_P_S_PRI, AmxOpCodeType.PackedOneParam },</v>
       </c>
     </row>
-    <row r="131" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A131" s="8">
         <v>129</v>
       </c>
@@ -5323,7 +5317,7 @@
         <v>{ AmxOpCode.LREF_P_S_ALT, AmxOpCodeType.PackedOneParam },</v>
       </c>
     </row>
-    <row r="132" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A132" s="8">
         <v>130</v>
       </c>
@@ -5349,7 +5343,7 @@
         <v>{ AmxOpCode.LODB_P_I, AmxOpCodeType.PackedOneParam },</v>
       </c>
     </row>
-    <row r="133" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133" s="8">
         <v>131</v>
       </c>
@@ -5375,7 +5369,7 @@
         <v>{ AmxOpCode.CONST_P_PRI, AmxOpCodeType.PackedOneParam },</v>
       </c>
     </row>
-    <row r="134" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134" s="8">
         <v>132</v>
       </c>
@@ -5401,7 +5395,7 @@
         <v>{ AmxOpCode.CONST_P_ALT, AmxOpCodeType.PackedOneParam },</v>
       </c>
     </row>
-    <row r="135" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135" s="8">
         <v>133</v>
       </c>
@@ -5427,7 +5421,7 @@
         <v>{ AmxOpCode.ADDR_P_PRI, AmxOpCodeType.PackedOneParam },</v>
       </c>
     </row>
-    <row r="136" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A136" s="8">
         <v>134</v>
       </c>
@@ -5453,7 +5447,7 @@
         <v>{ AmxOpCode.ADDR_P_ALT, AmxOpCodeType.PackedOneParam },</v>
       </c>
     </row>
-    <row r="137" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137" s="8">
         <v>135</v>
       </c>
@@ -5479,7 +5473,7 @@
         <v>{ AmxOpCode.STOR_P, AmxOpCodeType.PackedOneParam },</v>
       </c>
     </row>
-    <row r="138" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A138" s="8">
         <v>136</v>
       </c>
@@ -5505,7 +5499,7 @@
         <v>{ AmxOpCode.STOR_P_S, AmxOpCodeType.PackedOneParam },</v>
       </c>
     </row>
-    <row r="139" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A139" s="8">
         <v>137</v>
       </c>
@@ -5531,7 +5525,7 @@
         <v>{ AmxOpCode.SREF_P_S, AmxOpCodeType.PackedOneParam },</v>
       </c>
     </row>
-    <row r="140" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140" s="8">
         <v>138</v>
       </c>
@@ -5557,7 +5551,7 @@
         <v>{ AmxOpCode.STRB_P_I, AmxOpCodeType.PackedOneParam },</v>
       </c>
     </row>
-    <row r="141" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A141" s="8">
         <v>139</v>
       </c>
@@ -5583,7 +5577,7 @@
         <v>{ AmxOpCode.LIDX_P_B, AmxOpCodeType.PackedOneParam },</v>
       </c>
     </row>
-    <row r="142" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A142" s="8">
         <v>140</v>
       </c>
@@ -5609,7 +5603,7 @@
         <v>{ AmxOpCode.IDXADDR_P_B, AmxOpCodeType.PackedOneParam },</v>
       </c>
     </row>
-    <row r="143" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A143" s="8">
         <v>141</v>
       </c>
@@ -5635,7 +5629,7 @@
         <v>{ AmxOpCode.ALIGN_P_PRI, AmxOpCodeType.PackedOneParam },</v>
       </c>
     </row>
-    <row r="144" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A144" s="8">
         <v>142</v>
       </c>
@@ -5661,7 +5655,7 @@
         <v>{ AmxOpCode.PUSH_P_C, AmxOpCodeType.PackedOneParam },</v>
       </c>
     </row>
-    <row r="145" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A145" s="8">
         <v>143</v>
       </c>
@@ -5687,7 +5681,7 @@
         <v>{ AmxOpCode.PUSH_P, AmxOpCodeType.PackedOneParam },</v>
       </c>
     </row>
-    <row r="146" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A146" s="8">
         <v>144</v>
       </c>
@@ -5713,7 +5707,7 @@
         <v>{ AmxOpCode.PUSH_P_S, AmxOpCodeType.PackedOneParam },</v>
       </c>
     </row>
-    <row r="147" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A147" s="8">
         <v>145</v>
       </c>
@@ -5739,7 +5733,7 @@
         <v>{ AmxOpCode.PUSH_P_ADR, AmxOpCodeType.PackedOneParam },</v>
       </c>
     </row>
-    <row r="148" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A148" s="8">
         <v>146</v>
       </c>
@@ -5765,7 +5759,7 @@
         <v>{ AmxOpCode.PUSHR_P_C, AmxOpCodeType.PackedOneParam },</v>
       </c>
     </row>
-    <row r="149" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A149" s="8">
         <v>147</v>
       </c>
@@ -5791,7 +5785,7 @@
         <v>{ AmxOpCode.PUSHR_P_S, AmxOpCodeType.PackedOneParam },</v>
       </c>
     </row>
-    <row r="150" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A150" s="8">
         <v>148</v>
       </c>
@@ -5817,7 +5811,7 @@
         <v>{ AmxOpCode.PUSHR_P_ADR, AmxOpCodeType.PackedOneParam },</v>
       </c>
     </row>
-    <row r="151" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A151" s="8">
         <v>149</v>
       </c>
@@ -5846,7 +5840,7 @@
         <v>{ AmxOpCode.PUSHM_P_C, AmxOpCodeType.PackedNParams },</v>
       </c>
     </row>
-    <row r="152" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A152" s="8">
         <v>150</v>
       </c>
@@ -5875,7 +5869,7 @@
         <v>{ AmxOpCode.PUSHM_P, AmxOpCodeType.PackedNParams },</v>
       </c>
     </row>
-    <row r="153" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A153" s="8">
         <v>151</v>
       </c>
@@ -5904,7 +5898,7 @@
         <v>{ AmxOpCode.PUSHM_P_S, AmxOpCodeType.PackedNParams },</v>
       </c>
     </row>
-    <row r="154" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A154" s="8">
         <v>152</v>
       </c>
@@ -5933,7 +5927,7 @@
         <v>{ AmxOpCode.PUSHM_P_ADR, AmxOpCodeType.PackedNParams },</v>
       </c>
     </row>
-    <row r="155" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A155" s="8">
         <v>153</v>
       </c>
@@ -5962,7 +5956,7 @@
         <v>{ AmxOpCode.PUSHRM_P_C, AmxOpCodeType.PackedNParams },</v>
       </c>
     </row>
-    <row r="156" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A156" s="8">
         <v>154</v>
       </c>
@@ -5991,7 +5985,7 @@
         <v>{ AmxOpCode.PUSHRM_P_S, AmxOpCodeType.PackedNParams },</v>
       </c>
     </row>
-    <row r="157" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A157" s="8">
         <v>155</v>
       </c>
@@ -6020,7 +6014,7 @@
         <v>{ AmxOpCode.PUSHRM_P_ADR, AmxOpCodeType.PackedNParams },</v>
       </c>
     </row>
-    <row r="158" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A158" s="8">
         <v>156</v>
       </c>
@@ -6046,7 +6040,7 @@
         <v>{ AmxOpCode.STACK_P, AmxOpCodeType.PackedOneParam },</v>
       </c>
     </row>
-    <row r="159" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A159" s="8">
         <v>157</v>
       </c>
@@ -6072,7 +6066,7 @@
         <v>{ AmxOpCode.HEAP_P, AmxOpCodeType.PackedOneParam },</v>
       </c>
     </row>
-    <row r="160" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A160" s="8">
         <v>158</v>
       </c>
@@ -6098,7 +6092,7 @@
         <v>{ AmxOpCode.SHL_P_C_PRI, AmxOpCodeType.PackedOneParam },</v>
       </c>
     </row>
-    <row r="161" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A161" s="8">
         <v>159</v>
       </c>
@@ -6124,7 +6118,7 @@
         <v>{ AmxOpCode.SHL_P_C_ALT, AmxOpCodeType.PackedOneParam },</v>
       </c>
     </row>
-    <row r="162" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A162" s="8">
         <v>160</v>
       </c>
@@ -6150,7 +6144,7 @@
         <v>{ AmxOpCode.ADD_P_C, AmxOpCodeType.PackedOneParam },</v>
       </c>
     </row>
-    <row r="163" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A163" s="8">
         <v>161</v>
       </c>
@@ -6176,7 +6170,7 @@
         <v>{ AmxOpCode.SMUL_P_C, AmxOpCodeType.PackedOneParam },</v>
       </c>
     </row>
-    <row r="164" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A164" s="8">
         <v>162</v>
       </c>
@@ -6202,7 +6196,7 @@
         <v>{ AmxOpCode.ZERO_P, AmxOpCodeType.PackedOneParam },</v>
       </c>
     </row>
-    <row r="165" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A165" s="8">
         <v>163</v>
       </c>
@@ -6228,7 +6222,7 @@
         <v>{ AmxOpCode.ZERO_P_S, AmxOpCodeType.PackedOneParam },</v>
       </c>
     </row>
-    <row r="166" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A166" s="8">
         <v>164</v>
       </c>
@@ -6254,7 +6248,7 @@
         <v>{ AmxOpCode.EQ_P_C_PRI, AmxOpCodeType.PackedOneParam },</v>
       </c>
     </row>
-    <row r="167" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A167" s="8">
         <v>165</v>
       </c>
@@ -6280,7 +6274,7 @@
         <v>{ AmxOpCode.EQ_P_C_ALT, AmxOpCodeType.PackedOneParam },</v>
       </c>
     </row>
-    <row r="168" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A168" s="8">
         <v>166</v>
       </c>
@@ -6306,7 +6300,7 @@
         <v>{ AmxOpCode.INC_P, AmxOpCodeType.PackedOneParam },</v>
       </c>
     </row>
-    <row r="169" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A169" s="8">
         <v>167</v>
       </c>
@@ -6332,7 +6326,7 @@
         <v>{ AmxOpCode.INC_P_S, AmxOpCodeType.PackedOneParam },</v>
       </c>
     </row>
-    <row r="170" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A170" s="8">
         <v>168</v>
       </c>
@@ -6358,7 +6352,7 @@
         <v>{ AmxOpCode.DEC_P, AmxOpCodeType.PackedOneParam },</v>
       </c>
     </row>
-    <row r="171" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A171" s="8">
         <v>169</v>
       </c>
@@ -6384,7 +6378,7 @@
         <v>{ AmxOpCode.DEC_P_S, AmxOpCodeType.PackedOneParam },</v>
       </c>
     </row>
-    <row r="172" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A172" s="8">
         <v>170</v>
       </c>
@@ -6410,7 +6404,7 @@
         <v>{ AmxOpCode.MOVS_P, AmxOpCodeType.PackedOneParam },</v>
       </c>
     </row>
-    <row r="173" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A173" s="8">
         <v>171</v>
       </c>
@@ -6436,7 +6430,7 @@
         <v>{ AmxOpCode.CMPS_P, AmxOpCodeType.PackedOneParam },</v>
       </c>
     </row>
-    <row r="174" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A174" s="8">
         <v>172</v>
       </c>
@@ -6462,7 +6456,7 @@
         <v>{ AmxOpCode.FILL_P, AmxOpCodeType.PackedOneParam },</v>
       </c>
     </row>
-    <row r="175" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A175" s="8">
         <v>173</v>
       </c>
@@ -6488,7 +6482,7 @@
         <v>{ AmxOpCode.HALT_P, AmxOpCodeType.PackedOneParam },</v>
       </c>
     </row>
-    <row r="176" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A176" s="8">
         <v>174</v>
       </c>

</xml_diff>